<commit_message>
Bug Fixes to Magazine. Added toasts and Additional beautification.
</commit_message>
<xml_diff>
--- a/migrations/Kannada Books.xlsx
+++ b/migrations/Kannada Books.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
   <si>
     <t>B18447</t>
   </si>
@@ -30,9 +30,6 @@
     <t>C-1,S1</t>
   </si>
   <si>
-    <t xml:space="preserve">Kannada </t>
-  </si>
-  <si>
     <t>B22874</t>
   </si>
   <si>
@@ -160,14 +157,49 @@
   </si>
   <si>
     <t>Yashassinatha payana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sl.No </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc .No </t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Storage Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject </t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Kannada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -189,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,16 +244,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,352 +573,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F17"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>4</v>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -882,7 +1006,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -894,7 +1018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>